<commit_message>
Started assimilating dataset from Costello for realistic kinematics
</commit_message>
<xml_diff>
--- a/dataset_01_medusae/deformedShapeHistory_Costello2020_fig9.xlsx
+++ b/dataset_01_medusae/deformedShapeHistory_Costello2020_fig9.xlsx
@@ -3611,8 +3611,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X30" sqref="X30"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="W27" sqref="W27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>